<commit_message>
Implemented with ArrayList<Integer>. Cut time by ~60%.
</commit_message>
<xml_diff>
--- a/Unit 7 Examples/DynamicArrayOfInt_time-estimates.xlsx
+++ b/Unit 7 Examples/DynamicArrayOfInt_time-estimates.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10575" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="v1.1 ArrayList&lt;Integer&gt;" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>time</t>
   </si>
@@ -517,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1404,7 +1405,7 @@
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="3">
-        <f t="shared" ref="E19:M19" si="11">SUM(F2:F18)</f>
+        <f t="shared" ref="F19:M19" si="11">SUM(F2:F18)</f>
         <v>1971365084282.5994</v>
       </c>
       <c r="G19" s="4">
@@ -1434,6 +1435,919 @@
       <c r="M19" s="5">
         <f t="shared" si="11"/>
         <v>62.468789904257591</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.86328125" customWidth="1"/>
+    <col min="5" max="5" width="11.06640625" customWidth="1"/>
+    <col min="6" max="13" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="12">
+        <f>3+122+39</f>
+        <v>164</v>
+      </c>
+      <c r="B2">
+        <f>LOG(A2,2)</f>
+        <v>7.3575520046180847</v>
+      </c>
+      <c r="C2" s="12">
+        <f>2^D2</f>
+        <v>32768</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <f>_xlfn.FORECAST.LINEAR(D2,B$2:B$7,D$2:D$7)</f>
+        <v>7.2180157095681601</v>
+      </c>
+      <c r="F2" s="6">
+        <f>2^E2</f>
+        <v>148.88098648074393</v>
+      </c>
+      <c r="G2" s="7">
+        <f>F2/1000</f>
+        <v>0.14888098648074394</v>
+      </c>
+      <c r="H2" s="7">
+        <f>G2/60</f>
+        <v>2.4813497746790656E-3</v>
+      </c>
+      <c r="I2" s="7">
+        <f>H2/60</f>
+        <v>4.1355829577984425E-5</v>
+      </c>
+      <c r="J2" s="7">
+        <f>I2/24</f>
+        <v>1.723159565749351E-6</v>
+      </c>
+      <c r="K2" s="7">
+        <f>J2/7</f>
+        <v>2.4616565224990727E-7</v>
+      </c>
+      <c r="L2" s="7">
+        <f>J2/(365.25/12)</f>
+        <v>5.6613045281292849E-8</v>
+      </c>
+      <c r="M2" s="8">
+        <f>J2/365.25</f>
+        <v>4.7177537734410707E-9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="12">
+        <f>2+406+142</f>
+        <v>550</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B9" si="0">LOG(A3,2)</f>
+        <v>9.1032878084120217</v>
+      </c>
+      <c r="C3" s="12">
+        <f t="shared" ref="C3:C18" si="1">2^D3</f>
+        <v>65536</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E18" si="2">_xlfn.FORECAST.LINEAR(D3,B$2:B$7,D$2:D$7)</f>
+        <v>9.2091163420282349</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F18" si="3">2^E3</f>
+        <v>591.86172083261522</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G19" si="4">F3/1000</f>
+        <v>0.59186172083261523</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:I18" si="5">G3/60</f>
+        <v>9.8643620138769202E-3</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" si="5"/>
+        <v>1.6440603356461533E-4</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J18" si="6">I3/24</f>
+        <v>6.8502513985256385E-6</v>
+      </c>
+      <c r="K3" s="7">
+        <f t="shared" ref="K3:K18" si="7">J3/7</f>
+        <v>9.786073426465197E-7</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:L18" si="8">J3/(365.25/12)</f>
+        <v>2.2505959420207436E-7</v>
+      </c>
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M18" si="9">J3/365.25</f>
+        <v>1.8754966183506198E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="12">
+        <f>7+1514+631</f>
+        <v>2152</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>11.071462362556625</v>
+      </c>
+      <c r="C4" s="12">
+        <f t="shared" si="1"/>
+        <v>131072</v>
+      </c>
+      <c r="D4">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>11.200216974488306</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="3"/>
+        <v>2352.8880676260878</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="4"/>
+        <v>2.3528880676260879</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="5"/>
+        <v>3.9214801127101469E-2</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="5"/>
+        <v>6.5358001878502449E-4</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="6"/>
+        <v>2.7232500782709354E-5</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="7"/>
+        <v>3.8903572546727646E-6</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="8"/>
+        <v>8.9470228444219642E-7</v>
+      </c>
+      <c r="M4" s="8">
+        <f t="shared" si="9"/>
+        <v>7.4558523703516373E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="12">
+        <f>6+6322+3330</f>
+        <v>9658</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>13.237508748172656</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>13.191317606948381</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="3"/>
+        <v>9353.6751303821911</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="4"/>
+        <v>9.3536751303821912</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="5"/>
+        <v>0.15589458550636986</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="5"/>
+        <v>2.5982430917728312E-3</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="6"/>
+        <v>1.0826012882386797E-4</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="7"/>
+        <v>1.5465732689123994E-5</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="8"/>
+        <v>3.5568009469853952E-6</v>
+      </c>
+      <c r="M5" s="8">
+        <f t="shared" si="9"/>
+        <v>2.964000789154496E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="12">
+        <f>13+25761+11917</f>
+        <v>37691</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>15.201932451970192</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" si="1"/>
+        <v>524288</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>15.182418239408456</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="3"/>
+        <v>37184.615642597651</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="4"/>
+        <v>37.184615642597649</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="5"/>
+        <v>0.61974359404329415</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="5"/>
+        <v>1.032905990072157E-2</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="6"/>
+        <v>4.3037749586339875E-4</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="7"/>
+        <v>6.1482499409056961E-5</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4139712389762587E-5</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1783093658135489E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="12">
+        <f>25+102032+48804</f>
+        <v>150861</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>17.202860368580492</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="1"/>
+        <v>1048576</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>17.173518871868531</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="3"/>
+        <v>147823.78276069346</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="4"/>
+        <v>147.82378276069346</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="5"/>
+        <v>2.4637297126782243</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="5"/>
+        <v>4.1062161877970405E-2</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="6"/>
+        <v>1.7109234115821003E-3</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="7"/>
+        <v>2.4441763022601431E-4</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="8"/>
+        <v>5.6211036109473519E-5</v>
+      </c>
+      <c r="M7" s="8">
+        <f t="shared" si="9"/>
+        <v>4.684253009122793E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C8" s="12">
+        <f t="shared" si="1"/>
+        <v>2097152</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>19.164619504328606</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="3"/>
+        <v>587658.91140872252</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="4"/>
+        <v>587.65891140872247</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="5"/>
+        <v>9.7943151901453742</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="5"/>
+        <v>0.1632385865024229</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="6"/>
+        <v>6.8016077709342872E-3</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="7"/>
+        <v>9.7165825299061243E-4</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="8"/>
+        <v>2.2346144627299506E-4</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" si="9"/>
+        <v>1.8621787189416255E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C9" s="12">
+        <f t="shared" si="1"/>
+        <v>4194304</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>21.15572013678868</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="3"/>
+        <v>2336180.2120647077</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="4"/>
+        <v>2336.1802120647076</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="5"/>
+        <v>38.936336867745126</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="5"/>
+        <v>0.64893894779575212</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="6"/>
+        <v>2.7039122824823004E-2</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="7"/>
+        <v>3.8627318321175718E-3</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="8"/>
+        <v>8.8834900451163876E-4</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" si="9"/>
+        <v>7.4029083709303221E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C10" s="12">
+        <f t="shared" si="1"/>
+        <v>8388608</v>
+      </c>
+      <c r="D10">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>23.146820769248748</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="3"/>
+        <v>9287254.6936445143</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="4"/>
+        <v>9287.2546936445142</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="5"/>
+        <v>154.78757822740857</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="5"/>
+        <v>2.5797929704568094</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="6"/>
+        <v>0.10749137376903373</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="7"/>
+        <v>1.535591053843339E-2</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="8"/>
+        <v>3.5315441074015188E-3</v>
+      </c>
+      <c r="M10" s="8">
+        <f t="shared" si="9"/>
+        <v>2.942953422834599E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C11" s="12">
+        <f t="shared" si="1"/>
+        <v>16777216</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>25.137921401708823</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="3"/>
+        <v>36920567.728117317</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="4"/>
+        <v>36920.567728117319</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="5"/>
+        <v>615.34279546862194</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="5"/>
+        <v>10.255713257810365</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="6"/>
+        <v>0.42732138574209855</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="7"/>
+        <v>6.1045912248871223E-2</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="8"/>
+        <v>1.4039306307748618E-2</v>
+      </c>
+      <c r="M11" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1699421923123848E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C12" s="12">
+        <f t="shared" si="1"/>
+        <v>33554432</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>27.129022034168898</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="3"/>
+        <v>146774086.24308735</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="4"/>
+        <v>146774.08624308734</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="5"/>
+        <v>2446.2347707181225</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="5"/>
+        <v>40.770579511968705</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="6"/>
+        <v>1.6987741463320294</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="7"/>
+        <v>0.24268202090457563</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="8"/>
+        <v>5.5811881604337719E-2</v>
+      </c>
+      <c r="M12" s="8">
+        <f t="shared" si="9"/>
+        <v>4.6509901336948102E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C13" s="12">
+        <f t="shared" si="1"/>
+        <v>67108864</v>
+      </c>
+      <c r="D13">
+        <v>26</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>29.120122666628973</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="3"/>
+        <v>583485946.12989092</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="4"/>
+        <v>583485.94612989097</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="5"/>
+        <v>9724.7657688315157</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="5"/>
+        <v>162.07942948052525</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="6"/>
+        <v>6.7533095616885523</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="7"/>
+        <v>0.96475850881265035</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="8"/>
+        <v>0.22187464679058899</v>
+      </c>
+      <c r="M13" s="8">
+        <f t="shared" si="9"/>
+        <v>1.8489553899215749E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C14" s="12">
+        <f t="shared" si="1"/>
+        <v>134217728</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>31.111223299089048</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="3"/>
+        <v>2319590998.9671516</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="4"/>
+        <v>2319590.9989671516</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="5"/>
+        <v>38659.849982785861</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="5"/>
+        <v>644.33083304643105</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="6"/>
+        <v>26.847118043601295</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="7"/>
+        <v>3.8353025776573277</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="8"/>
+        <v>0.8820408392148269</v>
+      </c>
+      <c r="M14" s="8">
+        <f t="shared" si="9"/>
+        <v>7.3503403267902251E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C15" s="12">
+        <f t="shared" si="1"/>
+        <v>268435456</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>33.102323931549122</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="3"/>
+        <v>9221305908.3545876</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="4"/>
+        <v>9221305.9083545879</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="5"/>
+        <v>153688.43180590979</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="5"/>
+        <v>2561.4738634318296</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="6"/>
+        <v>106.7280776429929</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="7"/>
+        <v>15.246868234713272</v>
+      </c>
+      <c r="L15" s="7">
+        <f t="shared" si="8"/>
+        <v>3.5064666166075695</v>
+      </c>
+      <c r="M15" s="8">
+        <f t="shared" si="9"/>
+        <v>0.29220555138396415</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C16" s="12">
+        <f t="shared" si="1"/>
+        <v>536870912</v>
+      </c>
+      <c r="D16">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>35.09342456400919</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="3"/>
+        <v>36658394817.585159</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="4"/>
+        <v>36658394.817585163</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="5"/>
+        <v>610973.24695975275</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="5"/>
+        <v>10182.887449329213</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="6"/>
+        <v>424.28697705538389</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="7"/>
+        <v>60.612425293626266</v>
+      </c>
+      <c r="L16" s="7">
+        <f t="shared" si="8"/>
+        <v>13.939613209211791</v>
+      </c>
+      <c r="M16" s="8">
+        <f t="shared" si="9"/>
+        <v>1.1616344341009825</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="C17" s="12">
+        <f t="shared" si="1"/>
+        <v>1073741824</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>37.084525196469265</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="3"/>
+        <v>145731843619.28983</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="4"/>
+        <v>145731843.61928982</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="5"/>
+        <v>2428864.0603214968</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="5"/>
+        <v>40481.067672024947</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="6"/>
+        <v>1686.7111530010395</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="7"/>
+        <v>240.95873614300564</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="8"/>
+        <v>55.415561494900679</v>
+      </c>
+      <c r="M17" s="8">
+        <f t="shared" si="9"/>
+        <v>4.6179634579083899</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="C18" s="12">
+        <f t="shared" si="1"/>
+        <v>2147483648</v>
+      </c>
+      <c r="D18">
+        <v>31</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>39.07562582892934</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="3"/>
+        <v>579342613072.88086</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="4"/>
+        <v>579342613.07288086</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="5"/>
+        <v>9655710.217881348</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="5"/>
+        <v>160928.50363135579</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="6"/>
+        <v>6705.3543179731578</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="7"/>
+        <v>957.90775971045116</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="8"/>
+        <v>220.29911516954934</v>
+      </c>
+      <c r="M18" s="8">
+        <f t="shared" si="9"/>
+        <v>18.358259597462443</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3">
+        <f t="shared" ref="F19:M19" si="10">SUM(F2:F18)</f>
+        <v>774053337566.70007</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="4"/>
+        <v>774053337.5667001</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="10"/>
+        <v>12900888.959445002</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="10"/>
+        <v>215014.81599075004</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="10"/>
+        <v>8958.950666281251</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="10"/>
+        <v>1279.8500951830358</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="10"/>
+        <v>294.3392416026694</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="10"/>
+        <v>24.528270133555786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed final uses of DynamicArrayOfInt(). Now it's all ArrayList.
</commit_message>
<xml_diff>
--- a/Unit 7 Examples/DynamicArrayOfInt_time-estimates.xlsx
+++ b/Unit 7 Examples/DynamicArrayOfInt_time-estimates.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10575" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="v1.0" sheetId="1" r:id="rId1"/>
-    <sheet name="v1.1 ArrayList&lt;Integer&gt;" sheetId="2" r:id="rId2"/>
+    <sheet name="v1.0 - 62yrs" sheetId="1" r:id="rId1"/>
+    <sheet name="v1.1 - presumaby around 50yrs" sheetId="2" r:id="rId2"/>
+    <sheet name="v1.2 - 37yrs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
   <si>
     <t>time</t>
   </si>
@@ -1448,7 +1449,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2354,4 +2355,933 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.86328125" customWidth="1"/>
+    <col min="5" max="5" width="11.06640625" customWidth="1"/>
+    <col min="6" max="13" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" s="12">
+        <f>47*2</f>
+        <v>94</v>
+      </c>
+      <c r="B2">
+        <f>LOG(A2,2)</f>
+        <v>6.5545888516776376</v>
+      </c>
+      <c r="C2" s="12">
+        <f>2^D2</f>
+        <v>32768</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <f>_xlfn.FORECAST.LINEAR(D2,B$2:B$9,D$2:D$9)</f>
+        <v>6.295013088709176</v>
+      </c>
+      <c r="F2" s="6">
+        <f>2^E2</f>
+        <v>78.521350918262314</v>
+      </c>
+      <c r="G2" s="7">
+        <f>F2/1000</f>
+        <v>7.8521350918262317E-2</v>
+      </c>
+      <c r="H2" s="7">
+        <f>G2/60</f>
+        <v>1.3086891819710385E-3</v>
+      </c>
+      <c r="I2" s="7">
+        <f>H2/60</f>
+        <v>2.1811486366183976E-5</v>
+      </c>
+      <c r="J2" s="7">
+        <f>I2/24</f>
+        <v>9.0881193192433229E-7</v>
+      </c>
+      <c r="K2" s="7">
+        <f>J2/7</f>
+        <v>1.2983027598919034E-7</v>
+      </c>
+      <c r="L2" s="7">
+        <f>J2/(365.25/12)</f>
+        <v>2.9858297558088946E-8</v>
+      </c>
+      <c r="M2" s="8">
+        <f>J2/365.25</f>
+        <v>2.4881914631740787E-9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" s="12">
+        <f>172+171</f>
+        <v>343</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B9" si="0">LOG(A3,2)</f>
+        <v>8.4220647661728112</v>
+      </c>
+      <c r="C3" s="12">
+        <f t="shared" ref="C3:C18" si="1">2^D3</f>
+        <v>65536</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <f>_xlfn.FORECAST.LINEAR(D3,B$2:B$9,D$2:D$9)</f>
+        <v>8.3831953772863912</v>
+      </c>
+      <c r="F3" s="6">
+        <f t="shared" ref="F3:F18" si="2">2^E3</f>
+        <v>333.88220123358769</v>
+      </c>
+      <c r="G3" s="7">
+        <f t="shared" ref="G3:G19" si="3">F3/1000</f>
+        <v>0.33388220123358769</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" ref="H3:I18" si="4">G3/60</f>
+        <v>5.5647033538931282E-3</v>
+      </c>
+      <c r="I3" s="7">
+        <f t="shared" si="4"/>
+        <v>9.27450558982188E-5</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J18" si="5">I3/24</f>
+        <v>3.8643773290924503E-6</v>
+      </c>
+      <c r="K3" s="7">
+        <f t="shared" ref="K3:K18" si="6">J3/7</f>
+        <v>5.5205390415606428E-7</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:L18" si="7">J3/(365.25/12)</f>
+        <v>1.2696106214677454E-7</v>
+      </c>
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M18" si="8">J3/365.25</f>
+        <v>1.0580088512231212E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="12">
+        <f>641+641</f>
+        <v>1282</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>10.324180546618742</v>
+      </c>
+      <c r="C4" s="12">
+        <f t="shared" si="1"/>
+        <v>131072</v>
+      </c>
+      <c r="D4">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E3:E18" si="9">_xlfn.FORECAST.LINEAR(D4,B$2:B$9,D$2:D$9)</f>
+        <v>10.471377665863606</v>
+      </c>
+      <c r="F4" s="6">
+        <f t="shared" si="2"/>
+        <v>1419.7071624077066</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" si="3"/>
+        <v>1.4197071624077067</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" si="4"/>
+        <v>2.3661786040128443E-2</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" si="4"/>
+        <v>3.9436310066880739E-4</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="5"/>
+        <v>1.6431795861200309E-5</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="6"/>
+        <v>2.3473994087429014E-6</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="7"/>
+        <v>5.398536627909752E-7</v>
+      </c>
+      <c r="M4" s="8">
+        <f t="shared" si="8"/>
+        <v>4.4987805232581271E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" s="12">
+        <f>2793+2751</f>
+        <v>5544</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>12.436711542137214</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="9"/>
+        <v>12.559559954440822</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" si="2"/>
+        <v>6036.7651211860439</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="3"/>
+        <v>6.0367651211860442</v>
+      </c>
+      <c r="H5" s="7">
+        <f t="shared" si="4"/>
+        <v>0.10061275201976741</v>
+      </c>
+      <c r="I5" s="7">
+        <f t="shared" si="4"/>
+        <v>1.6768792003294568E-3</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="5"/>
+        <v>6.9869966680394035E-5</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="6"/>
+        <v>9.9814238114848619E-6</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="7"/>
+        <v>2.2955225192737258E-6</v>
+      </c>
+      <c r="M5" s="8">
+        <f t="shared" si="8"/>
+        <v>1.9129354327281049E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" s="12">
+        <f>15+11833+11643</f>
+        <v>23491</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>14.519820509005694</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" si="1"/>
+        <v>524288</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="9"/>
+        <v>14.647742243018037</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="2"/>
+        <v>25669.049289407576</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="3"/>
+        <v>25.669049289407575</v>
+      </c>
+      <c r="H6" s="7">
+        <f t="shared" si="4"/>
+        <v>0.42781748815679294</v>
+      </c>
+      <c r="I6" s="7">
+        <f t="shared" si="4"/>
+        <v>7.1302914692798819E-3</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="5"/>
+        <v>2.9709547788666176E-4</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="6"/>
+        <v>4.2442211126665966E-5</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="7"/>
+        <v>9.7608370558246171E-6</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="8"/>
+        <v>8.1340308798538465E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" s="12">
+        <f>16+48711+47524</f>
+        <v>96251</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>16.554513909205873</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="1"/>
+        <v>1048576</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="9"/>
+        <v>16.735924531595252</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="2"/>
+        <v>109147.87608840746</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="3"/>
+        <v>109.14787608840746</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="4"/>
+        <v>1.8191312681401244</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" si="4"/>
+        <v>3.0318854469002073E-2</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="5"/>
+        <v>1.2632856028750863E-3</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="6"/>
+        <v>1.8046937183929804E-4</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="7"/>
+        <v>4.1504249786450476E-5</v>
+      </c>
+      <c r="M7" s="8">
+        <f t="shared" si="8"/>
+        <v>3.4586874822042062E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" s="12">
+        <f>62+222730+217416</f>
+        <v>440208</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>18.747825838329284</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="1"/>
+        <v>2097152</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="9"/>
+        <v>18.824106820172474</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="2"/>
+        <v>464109.85932098713</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="3"/>
+        <v>464.10985932098714</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="4"/>
+        <v>7.7351643220164528</v>
+      </c>
+      <c r="I8" s="7">
+        <f t="shared" si="4"/>
+        <v>0.12891940536694088</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="5"/>
+        <v>5.3716418902892034E-3</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="6"/>
+        <v>7.6737741289845758E-4</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="7"/>
+        <v>1.7648104773024077E-4</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" si="8"/>
+        <v>1.4706753977520064E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" s="12">
+        <f>125+1270821+1256945</f>
+        <v>2527891</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>21.269502826688196</v>
+      </c>
+      <c r="C9" s="12">
+        <f t="shared" si="1"/>
+        <v>4194304</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="9"/>
+        <v>20.91228910874969</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="2"/>
+        <v>1973450.7829037106</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="3"/>
+        <v>1973.4507829037107</v>
+      </c>
+      <c r="H9" s="7">
+        <f t="shared" si="4"/>
+        <v>32.890846381728508</v>
+      </c>
+      <c r="I9" s="7">
+        <f t="shared" si="4"/>
+        <v>0.54818077302880852</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="5"/>
+        <v>2.2840865542867021E-2</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="6"/>
+        <v>3.2629807918381458E-3</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="7"/>
+        <v>7.5041858046380353E-4</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" si="8"/>
+        <v>6.253488170531696E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C10" s="12">
+        <f t="shared" si="1"/>
+        <v>8388608</v>
+      </c>
+      <c r="D10">
+        <v>23</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="9"/>
+        <v>23.000471397326905</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="2"/>
+        <v>8391349.4064554237</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="3"/>
+        <v>8391.3494064554234</v>
+      </c>
+      <c r="H10" s="7">
+        <f t="shared" si="4"/>
+        <v>139.85582344092373</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="4"/>
+        <v>2.3309303906820622</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="5"/>
+        <v>9.7122099611752596E-2</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="6"/>
+        <v>1.3874585658821799E-2</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="7"/>
+        <v>3.1908698024395105E-3</v>
+      </c>
+      <c r="M10" s="8">
+        <f t="shared" si="8"/>
+        <v>2.6590581686995919E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C11" s="12">
+        <f t="shared" si="1"/>
+        <v>16777216</v>
+      </c>
+      <c r="D11">
+        <v>24</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="9"/>
+        <v>25.08865368590412</v>
+      </c>
+      <c r="F11" s="6">
+        <f t="shared" si="2"/>
+        <v>35681024.057571024</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="3"/>
+        <v>35681.024057571027</v>
+      </c>
+      <c r="H11" s="7">
+        <f t="shared" si="4"/>
+        <v>594.68373429285043</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="4"/>
+        <v>9.9113955715475068</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="5"/>
+        <v>0.41297481548114612</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="6"/>
+        <v>5.8996402211592303E-2</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="7"/>
+        <v>1.3567961083569483E-2</v>
+      </c>
+      <c r="M11" s="8">
+        <f t="shared" si="8"/>
+        <v>1.1306634236307902E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C12" s="12">
+        <f t="shared" si="1"/>
+        <v>33554432</v>
+      </c>
+      <c r="D12">
+        <v>25</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="9"/>
+        <v>27.176835974481335</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="2"/>
+        <v>151719993.54687166</v>
+      </c>
+      <c r="G12" s="7">
+        <f t="shared" si="3"/>
+        <v>151719.99354687167</v>
+      </c>
+      <c r="H12" s="7">
+        <f t="shared" si="4"/>
+        <v>2528.6665591145279</v>
+      </c>
+      <c r="I12" s="7">
+        <f t="shared" si="4"/>
+        <v>42.144442651908797</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="5"/>
+        <v>1.7560184438295332</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="6"/>
+        <v>0.25085977768993334</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="7"/>
+        <v>5.7692597743886104E-2</v>
+      </c>
+      <c r="M12" s="8">
+        <f t="shared" si="8"/>
+        <v>4.8077164786571747E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C13" s="12">
+        <f t="shared" si="1"/>
+        <v>67108864</v>
+      </c>
+      <c r="D13">
+        <v>26</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="9"/>
+        <v>29.26501826305855</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="2"/>
+        <v>645131608.46286166</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="3"/>
+        <v>645131.60846286162</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="4"/>
+        <v>10752.193474381027</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="4"/>
+        <v>179.20322457301711</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="5"/>
+        <v>7.4668010238757132</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="6"/>
+        <v>1.0666858605536733</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="7"/>
+        <v>0.2453158447269228</v>
+      </c>
+      <c r="M13" s="8">
+        <f t="shared" si="8"/>
+        <v>2.04429870605769E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C14" s="12">
+        <f t="shared" si="1"/>
+        <v>134217728</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="9"/>
+        <v>31.353200551635766</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="2"/>
+        <v>2743176970.3397751</v>
+      </c>
+      <c r="G14" s="7">
+        <f t="shared" si="3"/>
+        <v>2743176.9703397751</v>
+      </c>
+      <c r="H14" s="7">
+        <f t="shared" si="4"/>
+        <v>45719.616172329588</v>
+      </c>
+      <c r="I14" s="7">
+        <f t="shared" si="4"/>
+        <v>761.99360287215984</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="5"/>
+        <v>31.749733453006659</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="6"/>
+        <v>4.5356762075723802</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="7"/>
+        <v>1.0431123927065842</v>
+      </c>
+      <c r="M14" s="8">
+        <f t="shared" si="8"/>
+        <v>8.6926032725548691E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C15" s="12">
+        <f t="shared" si="1"/>
+        <v>268435456</v>
+      </c>
+      <c r="D15">
+        <v>28</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="9"/>
+        <v>33.441382840212988</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="2"/>
+        <v>11664317469.317972</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" si="3"/>
+        <v>11664317.469317973</v>
+      </c>
+      <c r="H15" s="7">
+        <f t="shared" si="4"/>
+        <v>194405.29115529955</v>
+      </c>
+      <c r="I15" s="7">
+        <f t="shared" si="4"/>
+        <v>3240.0881859216593</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="5"/>
+        <v>135.00367441340248</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="6"/>
+        <v>19.28623920191464</v>
+      </c>
+      <c r="L15" s="7">
+        <f t="shared" si="7"/>
+        <v>4.435438995101519</v>
+      </c>
+      <c r="M15" s="8">
+        <f t="shared" si="8"/>
+        <v>0.36961991625845991</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="C16" s="12">
+        <f t="shared" si="1"/>
+        <v>536870912</v>
+      </c>
+      <c r="D16">
+        <v>29</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="9"/>
+        <v>35.529565128790203</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="2"/>
+        <v>49598076790.570053</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="3"/>
+        <v>49598076.79057005</v>
+      </c>
+      <c r="H16" s="7">
+        <f t="shared" si="4"/>
+        <v>826634.61317616748</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="4"/>
+        <v>13777.243552936125</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="5"/>
+        <v>574.05181470567186</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="6"/>
+        <v>82.007402100810268</v>
+      </c>
+      <c r="L16" s="7">
+        <f t="shared" si="7"/>
+        <v>18.860018552958419</v>
+      </c>
+      <c r="M16" s="8">
+        <f t="shared" si="8"/>
+        <v>1.5716682127465349</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="C17" s="12">
+        <f t="shared" si="1"/>
+        <v>1073741824</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="9"/>
+        <v>37.617747417367418</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="2"/>
+        <v>210896970850.97607</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="3"/>
+        <v>210896970.85097608</v>
+      </c>
+      <c r="H17" s="7">
+        <f t="shared" si="4"/>
+        <v>3514949.5141829345</v>
+      </c>
+      <c r="I17" s="7">
+        <f t="shared" si="4"/>
+        <v>58582.491903048911</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="5"/>
+        <v>2440.9371626270381</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="6"/>
+        <v>348.70530894671975</v>
+      </c>
+      <c r="L17" s="7">
+        <f t="shared" si="7"/>
+        <v>80.195060784461205</v>
+      </c>
+      <c r="M17" s="8">
+        <f t="shared" si="8"/>
+        <v>6.6829217320384346</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.45">
+      <c r="C18" s="12">
+        <f t="shared" si="1"/>
+        <v>2147483648</v>
+      </c>
+      <c r="D18">
+        <v>31</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="9"/>
+        <v>39.705929705944634</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="2"/>
+        <v>896759213102.67432</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="3"/>
+        <v>896759213.10267437</v>
+      </c>
+      <c r="H18" s="7">
+        <f t="shared" si="4"/>
+        <v>14945986.885044573</v>
+      </c>
+      <c r="I18" s="7">
+        <f t="shared" si="4"/>
+        <v>249099.78141740954</v>
+      </c>
+      <c r="J18" s="7">
+        <f t="shared" si="5"/>
+        <v>10379.157559058731</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="6"/>
+        <v>1482.7367941512473</v>
+      </c>
+      <c r="L18" s="7">
+        <f t="shared" si="7"/>
+        <v>340.99901631404452</v>
+      </c>
+      <c r="M18" s="8">
+        <f t="shared" si="8"/>
+        <v>28.416584692837045</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="D19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="3">
+        <f t="shared" ref="F19:M19" si="10">SUM(F2:F18)</f>
+        <v>1172505259405.7954</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="3"/>
+        <v>1172505259.4057953</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="10"/>
+        <v>19541754.323429924</v>
+      </c>
+      <c r="I19" s="4">
+        <f t="shared" si="10"/>
+        <v>325695.90539049869</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="10"/>
+        <v>13570.662724604113</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="10"/>
+        <v>1938.6661035148736</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="10"/>
+        <v>445.85339546953963</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="10"/>
+        <v>37.154449622461641</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>